<commit_message>
Integrate seed experiment data and add new plots
Added section to the RMarkdown framework for seed experiments and genetic diversity, sourced the integration script, and updated 'Seed experiment integration.R' to include fecundity, viability, and mass analyses with new data imports, statistical tests, and ggplot-based visualizations. Also added a new raw figure (figura 6.svg) and updated the germination data file.
</commit_message>
<xml_diff>
--- a/Data/Germination.xlsx
+++ b/Data/Germination.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\00 - Projetos\Parapiqueria\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2EF814-04E0-47B2-A476-460114FB0B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F3ED8C-4480-40F3-9BD5-AF3835431570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2175" yWindow="615" windowWidth="9780" windowHeight="8790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Germination" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="45">
   <si>
     <t>Parapiqueria</t>
   </si>
@@ -90,9 +90,6 @@
   </si>
   <si>
     <t>A8</t>
-  </si>
-  <si>
-    <t>sd</t>
   </si>
   <si>
     <t>Date field</t>
@@ -601,7 +598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -613,15 +610,15 @@
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1"/>
       <c r="D2" s="2" t="s">
@@ -631,15 +628,15 @@
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -723,7 +720,7 @@
         <v>1</v>
       </c>
       <c r="AD5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AE5" t="s">
         <v>2</v>
@@ -738,16 +735,16 @@
         <v>5</v>
       </c>
       <c r="AI5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ5" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="AJ5" s="7" t="s">
+      <c r="AK5" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="AK5" s="8" t="s">
+      <c r="AL5" t="s">
         <v>34</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.25">
@@ -1502,7 +1499,7 @@
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AE12" s="11">
         <f>AVERAGE(AE5:AE11)</f>
@@ -1632,10 +1629,10 @@
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16">
         <v>3</v>
@@ -1719,7 +1716,7 @@
         <v>1</v>
       </c>
       <c r="AD16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AE16" t="s">
         <v>2</v>
@@ -1734,16 +1731,16 @@
         <v>5</v>
       </c>
       <c r="AI16" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ16" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="AJ16" s="7" t="s">
+      <c r="AK16" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="AK16" s="8" t="s">
+      <c r="AL16" t="s">
         <v>34</v>
-      </c>
-      <c r="AL16" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:38" x14ac:dyDescent="0.25">
@@ -2498,7 +2495,7 @@
     </row>
     <row r="23" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AE23" s="11">
         <f>AVERAGE(AE17:AE22)</f>
@@ -2551,45 +2548,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1"/>
       <c r="D2" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -2597,10 +2594,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" t="s">
         <v>44</v>
-      </c>
-      <c r="B9" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2669,7 +2666,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B18">
         <f>AVERAGE(B10:B17)</f>
@@ -2687,17 +2684,17 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" t="s">
         <v>44</v>
-      </c>
-      <c r="B23" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2766,7 +2763,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B32">
         <f>AVERAGE(B24:B31)</f>
@@ -2775,7 +2772,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B33">
         <f>_xlfn.STDEV.S(B24:B31)</f>
@@ -2788,6 +2785,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e5de5f80-8a20-4bde-9392-005e37b5595b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="c16ac0c4-b43d-4687-a36f-62aa7d816e1d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006D29EB3ABB86614A88729F03313DFB21" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a97f8c2152d3c64de56626c01b37b2a7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e5de5f80-8a20-4bde-9392-005e37b5595b" xmlns:ns3="c16ac0c4-b43d-4687-a36f-62aa7d816e1d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cd42359836cbf3596a5dc9b36d884065" ns2:_="" ns3:_="">
     <xsd:import namespace="e5de5f80-8a20-4bde-9392-005e37b5595b"/>
@@ -3002,27 +3019,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e5de5f80-8a20-4bde-9392-005e37b5595b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="c16ac0c4-b43d-4687-a36f-62aa7d816e1d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A783975-6313-4A4F-A3E5-C5370FB1B081}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{988F8215-7B35-4074-840F-98CB0FB91ABD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e5de5f80-8a20-4bde-9392-005e37b5595b"/>
+    <ds:schemaRef ds:uri="c16ac0c4-b43d-4687-a36f-62aa7d816e1d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81A4818C-DB35-4653-9A9A-D2034D6FA3A7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3039,23 +3055,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{988F8215-7B35-4074-840F-98CB0FB91ABD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e5de5f80-8a20-4bde-9392-005e37b5595b"/>
-    <ds:schemaRef ds:uri="c16ac0c4-b43d-4687-a36f-62aa7d816e1d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A783975-6313-4A4F-A3E5-C5370FB1B081}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>